<commit_message>
update markets_details file and add create table from reshatot
</commit_message>
<xml_diff>
--- a/Files/markets_deatails_pub.xlsx
+++ b/Files/markets_deatails_pub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zvi Amosi\Documents\Studies\Data_Engineer\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB76883-D590-47DC-B7FF-772693D159ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E3DF64-251B-4B82-A560-E41486093252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98CB7264-79F4-42A1-AAFD-D092D353E047}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>vendor_website</t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>reshet_num</t>
+  </si>
+  <si>
+    <t>user_name</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14:E15"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -541,100 +541,100 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>7290492000005</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>7290873255550</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>7290700100008</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>7290803800003</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1">
         <v>7290103152017</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>7290526500006</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>12345</v>
@@ -642,120 +642,120 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <v>7290639000004</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
         <v>7291059100008</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>7290644700005</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
         <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1">
         <v>7290058177776</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
         <v>25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1">
         <v>7290876100000</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1">
         <v>7290785400000</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1">
         <v>7290058140886</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1">
         <v>7291056200008</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add con to minio+add file check in zvi folder
</commit_message>
<xml_diff>
--- a/Files/markets_deatails_pub.xlsx
+++ b/Files/markets_deatails_pub.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zvi Amosi\Documents\Studies\Data_Engineer\final_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZAMOS\Dropbox\Data_Engineer\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6C982B-DB35-41EB-90D5-99608D4429B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBA67ED-052A-4088-A9D7-5D288E9276D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98CB7264-79F4-42A1-AAFD-D092D353E047}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{98CB7264-79F4-42A1-AAFD-D092D353E047}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>רשת חנויות רמי לוי שיווק השקמה 2006 בע"מ</t>
   </si>
   <si>
-    <t>RamiLevi </t>
-  </si>
-  <si>
     <t>סופר קופיקס</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>SuperCofixApp</t>
+  </si>
+  <si>
+    <t>RamiLevi</t>
   </si>
 </sst>
 </file>
@@ -524,36 +524,36 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -567,7 +567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -581,7 +581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -595,7 +595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -609,7 +609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -623,7 +623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -640,7 +640,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -654,7 +654,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -668,7 +668,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -685,7 +685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -702,7 +702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -716,7 +716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -730,7 +730,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -741,12 +741,12 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>32</v>
       </c>
       <c r="B15" s="1">
         <v>7291056200008</v>
@@ -755,7 +755,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>